<commit_message>
Dodanie imputacji, dla zabawy i testów - dziala. Czytac literature i neta i na dyzur.
dodano rady od Dr Szymkowiaka

Ulepszenie pliku z danymi, by R łapał braki danych
</commit_message>
<xml_diff>
--- a/ankiety_wino.xlsx
+++ b/ankiety_wino.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" tabRatio="927" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" tabRatio="927"/>
   </bookViews>
   <sheets>
     <sheet name="Wszystko ;)" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="9">
   <si>
     <t>Pyt 4</t>
   </si>
@@ -384,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -811,12 +811,6 @@
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
@@ -1422,9 +1416,6 @@
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
@@ -1512,15 +1503,6 @@
       <c r="C30">
         <v>12</v>
       </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
       <c r="G30">
         <v>1</v>
       </c>
@@ -1600,9 +1582,6 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
-        <v>8</v>
-      </c>
       <c r="J32">
         <v>2</v>
       </c>
@@ -2960,9 +2939,6 @@
       <c r="D68">
         <v>62</v>
       </c>
-      <c r="E68" t="s">
-        <v>8</v>
-      </c>
       <c r="F68">
         <v>2</v>
       </c>
@@ -2980,9 +2956,6 @@
       </c>
       <c r="L68">
         <v>2</v>
-      </c>
-      <c r="M68" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -3080,9 +3053,6 @@
       <c r="F71">
         <v>2</v>
       </c>
-      <c r="G71" t="s">
-        <v>8</v>
-      </c>
       <c r="H71">
         <v>1</v>
       </c>
@@ -3454,9 +3424,6 @@
       <c r="D81">
         <v>60</v>
       </c>
-      <c r="E81" t="s">
-        <v>8</v>
-      </c>
       <c r="F81">
         <v>2</v>
       </c>
@@ -3907,9 +3874,6 @@
       <c r="C93">
         <v>2</v>
       </c>
-      <c r="D93" t="s">
-        <v>8</v>
-      </c>
       <c r="E93">
         <v>80</v>
       </c>
@@ -4556,9 +4520,6 @@
       <c r="D110">
         <v>60</v>
       </c>
-      <c r="E110" t="s">
-        <v>8</v>
-      </c>
       <c r="F110">
         <v>1</v>
       </c>
@@ -4670,9 +4631,6 @@
       <c r="D113">
         <v>70</v>
       </c>
-      <c r="E113" t="s">
-        <v>8</v>
-      </c>
       <c r="F113">
         <v>2</v>
       </c>
@@ -4711,9 +4669,6 @@
       <c r="E114">
         <v>80</v>
       </c>
-      <c r="F114" t="s">
-        <v>8</v>
-      </c>
       <c r="G114">
         <v>1</v>
       </c>
@@ -4822,9 +4777,6 @@
       <c r="D117">
         <v>27</v>
       </c>
-      <c r="E117" t="s">
-        <v>8</v>
-      </c>
       <c r="F117">
         <v>2</v>
       </c>
@@ -5246,9 +5198,6 @@
       <c r="F128">
         <v>2</v>
       </c>
-      <c r="G128" t="s">
-        <v>8</v>
-      </c>
       <c r="H128">
         <v>1</v>
       </c>
@@ -5337,9 +5286,6 @@
       <c r="L130">
         <v>3</v>
       </c>
-      <c r="M130" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="131" spans="1:13">
       <c r="A131">
@@ -5359,9 +5305,6 @@
       </c>
       <c r="F131">
         <v>2</v>
-      </c>
-      <c r="G131" t="s">
-        <v>8</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -6976,8 +6919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M30" sqref="B2:M30"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>